<commit_message>
last changes to v1.8.2
</commit_message>
<xml_diff>
--- a/clcore/output/StructureDefinition-BundleCl.xlsx
+++ b/clcore/output/StructureDefinition-BundleCl.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1749" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1749" uniqueCount="228">
   <si>
     <t>Property</t>
   </si>
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.8.1</t>
+    <t>1.8.2</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-06-27T22:42:19-04:00</t>
+    <t>2023-09-01T14:45:29-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -149,6 +149,10 @@
   </si>
   <si>
     <t>A container for a collection of resources.</t>
+  </si>
+  <si>
+    <t>bdl-1:total only when a search or history {total.empty() or (type = 'searchset') or (type = 'history')}
+bdl-2:entry.search only when a search {entry.search.empty() or (type = 'searchset')}bdl-3:entry.request mandatory for batch/transaction/history, otherwise prohibited {entry.all(request.exists() = (%resource.type = 'batch' or %resource.type = 'transaction' or %resource.type = 'history'))}bdl-4:entry.response mandatory for batch-response/transaction-response/history, otherwise prohibited {entry.all(response.exists() = (%resource.type = 'batch-response' or %resource.type = 'transaction-response' or %resource.type = 'history'))}bdl-7:FullUrl must be unique in a bundle, or else entries with the same fullUrl must have different meta.versionId (except in history bundles) {(type = 'history') or entry.where(fullUrl.exists()).select(fullUrl&amp;resource.meta.versionId).isDistinct()}bdl-9:A document must have an identifier with a system and a value {type = 'document' implies (identifier.system.exists() and identifier.value.exists())}bdl-10:A document must have a date {type = 'document' implies (timestamp.hasValue())}bdl-11:A document must have a Composition as the first resource {type = 'document' implies entry.first().resource.is(Composition)}bdl-12:A message must have a MessageHeader as the first resource {type = 'message' implies entry.first().resource.is(MessageHeader)}</t>
   </si>
   <si>
     <t>N/A</t>
@@ -1195,16 +1199,16 @@
         <v>38</v>
       </c>
       <c r="AJ1" t="s" s="2">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="AK1" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AL1" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AM1" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AN1" t="s" s="2">
         <v>38</v>
@@ -1212,10 +1216,10 @@
     </row>
     <row r="2" hidden="true">
       <c r="A2" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s" s="2">
@@ -1226,7 +1230,7 @@
         <v>39</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H2" t="s" s="2">
         <v>38</v>
@@ -1235,19 +1239,19 @@
         <v>38</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M2" t="s" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N2" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="O2" s="2"/>
       <c r="P2" t="s" s="2">
@@ -1297,13 +1301,13 @@
         <v>38</v>
       </c>
       <c r="AF2" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AG2" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH2" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI2" t="s" s="2">
         <v>38</v>
@@ -1326,10 +1330,10 @@
     </row>
     <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" t="s" s="2">
@@ -1340,7 +1344,7 @@
         <v>39</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H3" t="s" s="2">
         <v>38</v>
@@ -1349,16 +1353,16 @@
         <v>38</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M3" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -1409,19 +1413,19 @@
         <v>38</v>
       </c>
       <c r="AF3" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AG3" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH3" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI3" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ3" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK3" t="s" s="2">
         <v>38</v>
@@ -1438,10 +1442,10 @@
     </row>
     <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s" s="2">
@@ -1452,28 +1456,28 @@
         <v>39</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H4" t="s" s="2">
         <v>38</v>
       </c>
       <c r="I4" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M4" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N4" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O4" s="2"/>
       <c r="P4" t="s" s="2">
@@ -1523,19 +1527,19 @@
         <v>38</v>
       </c>
       <c r="AF4" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AG4" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI4" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK4" t="s" s="2">
         <v>38</v>
@@ -1552,10 +1556,10 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s" s="2">
@@ -1566,7 +1570,7 @@
         <v>39</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H5" t="s" s="2">
         <v>38</v>
@@ -1578,16 +1582,16 @@
         <v>38</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N5" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" t="s" s="2">
@@ -1613,13 +1617,13 @@
         <v>38</v>
       </c>
       <c r="X5" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Y5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z5" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA5" t="s" s="2">
         <v>38</v>
@@ -1637,19 +1641,19 @@
         <v>38</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AG5" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI5" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK5" t="s" s="2">
         <v>38</v>
@@ -1666,10 +1670,10 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
@@ -1677,31 +1681,31 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H6" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I6" t="s" s="2">
         <v>38</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N6" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" t="s" s="2">
@@ -1751,19 +1755,19 @@
         <v>38</v>
       </c>
       <c r="AF6" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG6" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH6" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI6" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK6" t="s" s="2">
         <v>38</v>
@@ -1772,18 +1776,18 @@
         <v>38</v>
       </c>
       <c r="AM6" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AN6" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" t="s" s="2">
@@ -1791,31 +1795,31 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H7" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I7" t="s" s="2">
         <v>38</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N7" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" t="s" s="2">
@@ -1841,11 +1845,11 @@
         <v>38</v>
       </c>
       <c r="X7" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Y7" s="2"/>
       <c r="Z7" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AA7" t="s" s="2">
         <v>38</v>
@@ -1863,19 +1867,19 @@
         <v>38</v>
       </c>
       <c r="AF7" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AG7" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AH7" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI7" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ7" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK7" t="s" s="2">
         <v>38</v>
@@ -1887,15 +1891,15 @@
         <v>38</v>
       </c>
       <c r="AN7" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s" s="2">
@@ -1903,31 +1907,31 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G8" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H8" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I8" t="s" s="2">
         <v>38</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="N8" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" t="s" s="2">
@@ -1977,19 +1981,19 @@
         <v>38</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AG8" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH8" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI8" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ8" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK8" t="s" s="2">
         <v>38</v>
@@ -1998,18 +2002,18 @@
         <v>38</v>
       </c>
       <c r="AM8" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AN8" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s" s="2">
@@ -2020,7 +2024,7 @@
         <v>39</v>
       </c>
       <c r="G9" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H9" t="s" s="2">
         <v>38</v>
@@ -2029,19 +2033,19 @@
         <v>38</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N9" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" t="s" s="2">
@@ -2091,19 +2095,19 @@
         <v>38</v>
       </c>
       <c r="AF9" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AG9" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH9" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK9" t="s" s="2">
         <v>38</v>
@@ -2120,10 +2124,10 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" t="s" s="2">
@@ -2143,19 +2147,19 @@
         <v>38</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="N10" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="O10" s="2"/>
       <c r="P10" t="s" s="2">
@@ -2205,7 +2209,7 @@
         <v>38</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AG10" t="s" s="2">
         <v>39</v>
@@ -2217,7 +2221,7 @@
         <v>38</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK10" t="s" s="2">
         <v>38</v>
@@ -2234,10 +2238,10 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
@@ -2248,7 +2252,7 @@
         <v>39</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H11" t="s" s="2">
         <v>38</v>
@@ -2260,13 +2264,13 @@
         <v>38</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -2317,13 +2321,13 @@
         <v>38</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AG11" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH11" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI11" t="s" s="2">
         <v>38</v>
@@ -2335,7 +2339,7 @@
         <v>38</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AM11" t="s" s="2">
         <v>38</v>
@@ -2346,14 +2350,14 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" t="s" s="2">
@@ -2372,16 +2376,16 @@
         <v>38</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N12" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="O12" s="2"/>
       <c r="P12" t="s" s="2">
@@ -2431,7 +2435,7 @@
         <v>38</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AG12" t="s" s="2">
         <v>39</v>
@@ -2443,13 +2447,13 @@
         <v>38</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AK12" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AM12" t="s" s="2">
         <v>38</v>
@@ -2460,14 +2464,14 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" t="s" s="2">
@@ -2480,25 +2484,25 @@
         <v>38</v>
       </c>
       <c r="I13" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="N13" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="O13" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="P13" t="s" s="2">
         <v>38</v>
@@ -2547,7 +2551,7 @@
         <v>38</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>39</v>
@@ -2559,13 +2563,13 @@
         <v>38</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AK13" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AM13" t="s" s="2">
         <v>38</v>
@@ -2576,10 +2580,10 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -2587,10 +2591,10 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H14" t="s" s="2">
         <v>38</v>
@@ -2599,16 +2603,16 @@
         <v>38</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -2659,19 +2663,19 @@
         <v>38</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AG14" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AH14" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI14" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK14" t="s" s="2">
         <v>38</v>
@@ -2688,10 +2692,10 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
@@ -2699,10 +2703,10 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H15" t="s" s="2">
         <v>38</v>
@@ -2711,16 +2715,16 @@
         <v>38</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -2771,19 +2775,19 @@
         <v>38</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AG15" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AH15" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI15" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK15" t="s" s="2">
         <v>38</v>
@@ -2800,10 +2804,10 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
@@ -2811,28 +2815,28 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G16" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H16" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I16" t="s" s="2">
         <v>38</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -2883,7 +2887,7 @@
         <v>38</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>39</v>
@@ -2895,7 +2899,7 @@
         <v>38</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AK16" t="s" s="2">
         <v>38</v>
@@ -2912,10 +2916,10 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
@@ -2926,7 +2930,7 @@
         <v>39</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>38</v>
@@ -2938,13 +2942,13 @@
         <v>38</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
@@ -2995,13 +2999,13 @@
         <v>38</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH17" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI17" t="s" s="2">
         <v>38</v>
@@ -3013,7 +3017,7 @@
         <v>38</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AM17" t="s" s="2">
         <v>38</v>
@@ -3024,14 +3028,14 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" t="s" s="2">
@@ -3050,16 +3054,16 @@
         <v>38</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" t="s" s="2">
@@ -3109,7 +3113,7 @@
         <v>38</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>39</v>
@@ -3121,13 +3125,13 @@
         <v>38</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AK18" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AM18" t="s" s="2">
         <v>38</v>
@@ -3138,14 +3142,14 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" t="s" s="2">
@@ -3158,25 +3162,25 @@
         <v>38</v>
       </c>
       <c r="I19" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="O19" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="P19" t="s" s="2">
         <v>38</v>
@@ -3225,7 +3229,7 @@
         <v>38</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>39</v>
@@ -3237,13 +3241,13 @@
         <v>38</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AM19" t="s" s="2">
         <v>38</v>
@@ -3254,10 +3258,10 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -3277,16 +3281,16 @@
         <v>38</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K20" t="s" s="2">
         <v>41</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -3337,7 +3341,7 @@
         <v>38</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>39</v>
@@ -3349,7 +3353,7 @@
         <v>38</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK20" t="s" s="2">
         <v>38</v>
@@ -3366,10 +3370,10 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -3380,28 +3384,28 @@
         <v>39</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H21" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I21" t="s" s="2">
         <v>38</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" t="s" s="2">
@@ -3451,19 +3455,19 @@
         <v>38</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH21" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI21" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>38</v>
@@ -3480,10 +3484,10 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -3494,7 +3498,7 @@
         <v>39</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>38</v>
@@ -3503,16 +3507,16 @@
         <v>38</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -3563,13 +3567,13 @@
         <v>38</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI22" t="s" s="2">
         <v>38</v>
@@ -3592,10 +3596,10 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -3606,7 +3610,7 @@
         <v>39</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H23" t="s" s="2">
         <v>38</v>
@@ -3615,16 +3619,16 @@
         <v>38</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -3675,19 +3679,19 @@
         <v>38</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>38</v>
@@ -3704,10 +3708,10 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -3718,7 +3722,7 @@
         <v>39</v>
       </c>
       <c r="G24" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H24" t="s" s="2">
         <v>38</v>
@@ -3730,13 +3734,13 @@
         <v>38</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -3787,13 +3791,13 @@
         <v>38</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>38</v>
@@ -3805,7 +3809,7 @@
         <v>38</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AM24" t="s" s="2">
         <v>38</v>
@@ -3816,14 +3820,14 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" t="s" s="2">
@@ -3842,16 +3846,16 @@
         <v>38</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" t="s" s="2">
@@ -3901,7 +3905,7 @@
         <v>38</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>39</v>
@@ -3913,13 +3917,13 @@
         <v>38</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AK25" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AM25" t="s" s="2">
         <v>38</v>
@@ -3930,14 +3934,14 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" t="s" s="2">
@@ -3950,25 +3954,25 @@
         <v>38</v>
       </c>
       <c r="I26" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="O26" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>38</v>
@@ -4017,7 +4021,7 @@
         <v>38</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>39</v>
@@ -4029,13 +4033,13 @@
         <v>38</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AK26" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AM26" t="s" s="2">
         <v>38</v>
@@ -4046,10 +4050,10 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4060,7 +4064,7 @@
         <v>39</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>38</v>
@@ -4069,19 +4073,19 @@
         <v>38</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" t="s" s="2">
@@ -4107,13 +4111,13 @@
         <v>38</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="Z27" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AA27" t="s" s="2">
         <v>38</v>
@@ -4131,19 +4135,19 @@
         <v>38</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH27" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI27" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK27" t="s" s="2">
         <v>38</v>
@@ -4160,10 +4164,10 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4174,7 +4178,7 @@
         <v>39</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H28" t="s" s="2">
         <v>38</v>
@@ -4183,19 +4187,19 @@
         <v>38</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
@@ -4245,19 +4249,19 @@
         <v>38</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH28" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI28" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>38</v>
@@ -4274,10 +4278,10 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -4288,7 +4292,7 @@
         <v>39</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H29" t="s" s="2">
         <v>38</v>
@@ -4297,16 +4301,16 @@
         <v>38</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -4357,19 +4361,19 @@
         <v>38</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH29" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK29" t="s" s="2">
         <v>38</v>
@@ -4386,10 +4390,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -4400,7 +4404,7 @@
         <v>39</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H30" t="s" s="2">
         <v>38</v>
@@ -4412,13 +4416,13 @@
         <v>38</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -4469,13 +4473,13 @@
         <v>38</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH30" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI30" t="s" s="2">
         <v>38</v>
@@ -4487,7 +4491,7 @@
         <v>38</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AM30" t="s" s="2">
         <v>38</v>
@@ -4498,14 +4502,14 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s" s="2">
@@ -4524,16 +4528,16 @@
         <v>38</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" t="s" s="2">
@@ -4583,7 +4587,7 @@
         <v>38</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>39</v>
@@ -4595,13 +4599,13 @@
         <v>38</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AM31" t="s" s="2">
         <v>38</v>
@@ -4612,14 +4616,14 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" t="s" s="2">
@@ -4632,25 +4636,25 @@
         <v>38</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="O32" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="P32" t="s" s="2">
         <v>38</v>
@@ -4699,7 +4703,7 @@
         <v>38</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>39</v>
@@ -4711,13 +4715,13 @@
         <v>38</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AM32" t="s" s="2">
         <v>38</v>
@@ -4728,10 +4732,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -4739,10 +4743,10 @@
       </c>
       <c r="E33" s="2"/>
       <c r="F33" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G33" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H33" t="s" s="2">
         <v>38</v>
@@ -4751,16 +4755,16 @@
         <v>38</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -4787,13 +4791,13 @@
         <v>38</v>
       </c>
       <c r="X33" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Y33" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="Z33" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="AA33" t="s" s="2">
         <v>38</v>
@@ -4811,19 +4815,19 @@
         <v>38</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI33" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK33" t="s" s="2">
         <v>38</v>
@@ -4840,10 +4844,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -4851,10 +4855,10 @@
       </c>
       <c r="E34" s="2"/>
       <c r="F34" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>38</v>
@@ -4863,19 +4867,19 @@
         <v>38</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O34" s="2"/>
       <c r="P34" t="s" s="2">
@@ -4925,19 +4929,19 @@
         <v>38</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="AG34" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>38</v>
@@ -4954,10 +4958,10 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -4968,7 +4972,7 @@
         <v>39</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>38</v>
@@ -4977,16 +4981,16 @@
         <v>38</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -5037,19 +5041,19 @@
         <v>38</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>38</v>
@@ -5066,10 +5070,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5080,7 +5084,7 @@
         <v>39</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H36" t="s" s="2">
         <v>38</v>
@@ -5089,16 +5093,16 @@
         <v>38</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -5149,19 +5153,19 @@
         <v>38</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>38</v>
@@ -5178,10 +5182,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5192,7 +5196,7 @@
         <v>39</v>
       </c>
       <c r="G37" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H37" t="s" s="2">
         <v>38</v>
@@ -5201,16 +5205,16 @@
         <v>38</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -5261,19 +5265,19 @@
         <v>38</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>38</v>
@@ -5290,10 +5294,10 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -5304,7 +5308,7 @@
         <v>39</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>38</v>
@@ -5313,16 +5317,16 @@
         <v>38</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -5373,19 +5377,19 @@
         <v>38</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI38" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>38</v>
@@ -5402,10 +5406,10 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -5416,7 +5420,7 @@
         <v>39</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H39" t="s" s="2">
         <v>38</v>
@@ -5425,16 +5429,16 @@
         <v>38</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -5485,19 +5489,19 @@
         <v>38</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH39" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>38</v>
@@ -5514,10 +5518,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -5528,7 +5532,7 @@
         <v>39</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H40" t="s" s="2">
         <v>38</v>
@@ -5540,13 +5544,13 @@
         <v>38</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -5597,13 +5601,13 @@
         <v>38</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI40" t="s" s="2">
         <v>38</v>
@@ -5615,7 +5619,7 @@
         <v>38</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>38</v>
@@ -5626,14 +5630,14 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s" s="2">
@@ -5652,16 +5656,16 @@
         <v>38</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="O41" s="2"/>
       <c r="P41" t="s" s="2">
@@ -5711,7 +5715,7 @@
         <v>38</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>39</v>
@@ -5723,13 +5727,13 @@
         <v>38</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AK41" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>38</v>
@@ -5740,14 +5744,14 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" t="s" s="2">
@@ -5760,25 +5764,25 @@
         <v>38</v>
       </c>
       <c r="I42" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="O42" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="P42" t="s" s="2">
         <v>38</v>
@@ -5827,7 +5831,7 @@
         <v>38</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>39</v>
@@ -5839,13 +5843,13 @@
         <v>38</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AK42" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AM42" t="s" s="2">
         <v>38</v>
@@ -5856,10 +5860,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -5867,10 +5871,10 @@
       </c>
       <c r="E43" s="2"/>
       <c r="F43" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G43" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H43" t="s" s="2">
         <v>38</v>
@@ -5879,16 +5883,16 @@
         <v>38</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -5939,19 +5943,19 @@
         <v>38</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AH43" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI43" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>38</v>
@@ -5968,10 +5972,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -5982,7 +5986,7 @@
         <v>39</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H44" t="s" s="2">
         <v>38</v>
@@ -5991,16 +5995,16 @@
         <v>38</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -6051,19 +6055,19 @@
         <v>38</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH44" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI44" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK44" t="s" s="2">
         <v>38</v>
@@ -6080,10 +6084,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6094,7 +6098,7 @@
         <v>39</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H45" t="s" s="2">
         <v>38</v>
@@ -6103,19 +6107,19 @@
         <v>38</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
@@ -6165,19 +6169,19 @@
         <v>38</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH45" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI45" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>38</v>
@@ -6194,10 +6198,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -6208,7 +6212,7 @@
         <v>39</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H46" t="s" s="2">
         <v>38</v>
@@ -6217,19 +6221,19 @@
         <v>38</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
@@ -6279,19 +6283,19 @@
         <v>38</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH46" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI46" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK46" t="s" s="2">
         <v>38</v>
@@ -6308,10 +6312,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -6322,7 +6326,7 @@
         <v>39</v>
       </c>
       <c r="G47" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H47" t="s" s="2">
         <v>38</v>
@@ -6331,19 +6335,19 @@
         <v>38</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
@@ -6393,13 +6397,13 @@
         <v>38</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH47" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI47" t="s" s="2">
         <v>38</v>
@@ -6422,10 +6426,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -6436,7 +6440,7 @@
         <v>39</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>38</v>
@@ -6445,22 +6449,22 @@
         <v>38</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="O48" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="P48" t="s" s="2">
         <v>38</v>
@@ -6509,19 +6513,19 @@
         <v>38</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AH48" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI48" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK48" t="s" s="2">
         <v>38</v>

</xml_diff>